<commit_message>
burndownchart aktualisierung (iteration 5)
</commit_message>
<xml_diff>
--- a/Dokumentation/MS5/Burndown.xlsx
+++ b/Dokumentation/MS5/Burndown.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4470" windowWidth="15360" windowHeight="6315" tabRatio="646" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="4470" windowWidth="15360" windowHeight="6315" tabRatio="646" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Resource Allocation" sheetId="2" r:id="rId1"/>
@@ -625,8 +625,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.3824769903762037"/>
-          <c:y val="1.9575856443719432E-2"/>
+          <c:x val="0.38247699037620386"/>
+          <c:y val="1.9575856443719439E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -644,8 +644,8 @@
           <c:yMode val="edge"/>
           <c:x val="6.3263041065482792E-2"/>
           <c:y val="0.11092985318107668"/>
-          <c:w val="0.78912319644839191"/>
-          <c:h val="0.79282218597063447"/>
+          <c:w val="0.78912319644839202"/>
+          <c:h val="0.79282218597063436"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -780,16 +780,16 @@
                   <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14</c:v>
+                  <c:v>13.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.5</c:v>
+                  <c:v>11.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.5</c:v>
+                  <c:v>10.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.5</c:v>
+                  <c:v>10.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -817,11 +817,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="37006720"/>
-        <c:axId val="37021568"/>
+        <c:axId val="60530688"/>
+        <c:axId val="60533376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="37006720"/>
+        <c:axId val="60530688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -891,7 +891,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37021568"/>
+        <c:crossAx val="60533376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -900,7 +900,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="37021568"/>
+        <c:axId val="60533376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -943,7 +943,7 @@
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
               <c:x val="1.2208724689406945E-2"/>
-              <c:y val="0.43230022178461236"/>
+              <c:y val="0.43230022178461247"/>
             </c:manualLayout>
           </c:layout>
           <c:spPr>
@@ -980,7 +980,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37006720"/>
+        <c:crossAx val="60530688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1000,9 +1000,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.86459489650160981"/>
-          <c:y val="0.47634588537670086"/>
-          <c:w val="0.13096554606043787"/>
+          <c:x val="0.86459489650160992"/>
+          <c:y val="0.47634588537670092"/>
+          <c:w val="0.13096554606043792"/>
           <c:h val="6.3621571147249978E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -1124,8 +1124,8 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="88911232"/>
-        <c:axId val="37475456"/>
+        <c:axId val="60729600"/>
+        <c:axId val="60735488"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1214,11 +1214,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="88911232"/>
-        <c:axId val="37475456"/>
+        <c:axId val="60729600"/>
+        <c:axId val="60735488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="88911232"/>
+        <c:axId val="60729600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1242,14 +1242,14 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37475456"/>
+        <c:crossAx val="60735488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="37475456"/>
+        <c:axId val="60735488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1274,7 +1274,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88911232"/>
+        <c:crossAx val="60729600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1285,10 +1285,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.77880952380952551"/>
+          <c:x val="0.77880952380952573"/>
           <c:y val="0.38324174513150894"/>
           <c:w val="0.20690476190476192"/>
-          <c:h val="0.20622139015839858"/>
+          <c:h val="0.20622139015839863"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -1331,7 +1331,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1341,7 +1341,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Chart2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0"/>
+    <sheetView zoomScale="106" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -3539,19 +3539,19 @@
       </c>
       <c r="D4" s="11">
         <f ca="1"/>
-        <v>6</v>
+        <v>5.75</v>
       </c>
       <c r="E4" s="11">
         <f ca="1"/>
-        <v>6</v>
+        <v>5.25</v>
       </c>
       <c r="F4" s="11">
         <f ca="1"/>
-        <v>6</v>
+        <v>5.25</v>
       </c>
       <c r="G4" s="11">
         <f ca="1"/>
-        <v>6</v>
+        <v>5.25</v>
       </c>
       <c r="H4" s="11">
         <f ca="1"/>
@@ -5218,19 +5218,19 @@
       </c>
       <c r="D8" s="12">
         <f ca="1">IF('Sprint Information'!C$52,SUM(OFFSET(D$2,1,0,ROW()-3,1)),"")</f>
-        <v>14</v>
+        <v>13.75</v>
       </c>
       <c r="E8" s="12">
         <f ca="1">IF('Sprint Information'!D$52,SUM(OFFSET(E$2,1,0,ROW()-3,1)),"")</f>
-        <v>12.5</v>
+        <v>11.75</v>
       </c>
       <c r="F8" s="12">
         <f ca="1">IF('Sprint Information'!E$52,SUM(OFFSET(F$2,1,0,ROW()-3,1)),"")</f>
-        <v>11.5</v>
+        <v>10.75</v>
       </c>
       <c r="G8" s="12">
         <f ca="1">IF('Sprint Information'!F$52,SUM(OFFSET(G$2,1,0,ROW()-3,1)),"")</f>
-        <v>11.5</v>
+        <v>10.75</v>
       </c>
       <c r="H8" s="12">
         <f ca="1">IF('Sprint Information'!G$52,SUM(OFFSET(H$2,1,0,ROW()-3,1)),"")</f>
@@ -5656,7 +5656,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:DE23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -6580,21 +6580,35 @@
         <v>0.5</v>
       </c>
       <c r="I4" s="25">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="J4" s="25">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="K4" s="25">
-        <v>0.5</v>
-      </c>
-      <c r="L4" s="25"/>
-      <c r="M4" s="25"/>
-      <c r="N4" s="25"/>
-      <c r="O4" s="28"/>
-      <c r="P4" s="28"/>
-      <c r="Q4" s="28"/>
-      <c r="R4" s="28"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="25">
+        <v>0</v>
+      </c>
+      <c r="M4" s="25">
+        <v>0</v>
+      </c>
+      <c r="N4" s="25">
+        <v>0</v>
+      </c>
+      <c r="O4" s="28">
+        <v>0</v>
+      </c>
+      <c r="P4" s="28">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="28">
+        <v>0</v>
+      </c>
+      <c r="R4" s="28">
+        <v>0</v>
+      </c>
       <c r="S4" s="29"/>
       <c r="T4" s="29"/>
       <c r="U4" s="29"/>
@@ -7203,16 +7217,16 @@
         <v>5.5</v>
       </c>
       <c r="H19" s="25">
-        <v>5.5</v>
+        <v>5.25</v>
       </c>
       <c r="I19" s="25">
-        <v>5.5</v>
+        <v>5.25</v>
       </c>
       <c r="J19" s="25">
-        <v>5.5</v>
+        <v>5.25</v>
       </c>
       <c r="K19" s="25">
-        <v>5.5</v>
+        <v>5.25</v>
       </c>
       <c r="L19" s="25"/>
       <c r="M19" s="25"/>
@@ -9254,19 +9268,19 @@
       </c>
       <c r="E4" s="11">
         <f ca="1"/>
-        <v>6</v>
+        <v>5.75</v>
       </c>
       <c r="F4" s="11">
         <f ca="1"/>
-        <v>6</v>
+        <v>5.25</v>
       </c>
       <c r="G4" s="11">
         <f ca="1"/>
-        <v>6</v>
+        <v>5.25</v>
       </c>
       <c r="H4" s="11">
         <f ca="1"/>
-        <v>6</v>
+        <v>5.25</v>
       </c>
       <c r="I4" s="11">
         <f ca="1"/>
@@ -10958,19 +10972,19 @@
       </c>
       <c r="E8" s="11">
         <f ca="1"/>
-        <v>14</v>
+        <v>13.75</v>
       </c>
       <c r="F8" s="11">
         <f ca="1"/>
-        <v>12.5</v>
+        <v>11.75</v>
       </c>
       <c r="G8" s="11">
         <f ca="1"/>
-        <v>11.5</v>
+        <v>10.75</v>
       </c>
       <c r="H8" s="11">
         <f ca="1"/>
-        <v>11.5</v>
+        <v>10.75</v>
       </c>
       <c r="I8" s="11">
         <f ca="1"/>
@@ -24649,9 +24663,9 @@
       <c r="A60" t="s">
         <v>28</v>
       </c>
-      <c r="B60" t="e">
+      <c r="B60" t="str">
         <f ca="1">MID(CELL("filename"),FIND("[",CELL("filename"))+1,FIND("]",CELL("filename"))-FIND("[",CELL("filename"))-IF(MID(CELL("filename"),FIND("]",CELL("filename"))-4,1)=".",5,6))</f>
-        <v>#N/A</v>
+        <v>Burndown</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
burndownchart iteration 5 fertig
</commit_message>
<xml_diff>
--- a/Dokumentation/MS5/Burndown.xlsx
+++ b/Dokumentation/MS5/Burndown.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4470" windowWidth="15360" windowHeight="6315" tabRatio="646" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="4470" windowWidth="15360" windowHeight="6315" tabRatio="646" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Resource Allocation" sheetId="2" r:id="rId1"/>
@@ -391,7 +391,163 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="36">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="26"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="26"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="26"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="26"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="26"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="26"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="26"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="26"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="26"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="26"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="26"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="26"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="26"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -625,8 +781,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38247699037620386"/>
-          <c:y val="1.9575856443719439E-2"/>
+          <c:x val="0.38247699037620397"/>
+          <c:y val="1.9575856443719442E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -644,8 +800,8 @@
           <c:yMode val="edge"/>
           <c:x val="6.3263041065482792E-2"/>
           <c:y val="0.11092985318107668"/>
-          <c:w val="0.78912319644839202"/>
-          <c:h val="0.79282218597063436"/>
+          <c:w val="0.78912319644839213"/>
+          <c:h val="0.79282218597063425"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -792,36 +948,36 @@
                   <c:v>10.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>10.75</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="60530688"/>
-        <c:axId val="60533376"/>
+        <c:axId val="36675968"/>
+        <c:axId val="36678272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="60530688"/>
+        <c:axId val="36675968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -891,7 +1047,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60533376"/>
+        <c:crossAx val="36678272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -900,7 +1056,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60533376"/>
+        <c:axId val="36678272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -943,7 +1099,7 @@
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
               <c:x val="1.2208724689406945E-2"/>
-              <c:y val="0.43230022178461247"/>
+              <c:y val="0.43230022178461258"/>
             </c:manualLayout>
           </c:layout>
           <c:spPr>
@@ -980,7 +1136,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60530688"/>
+        <c:crossAx val="36675968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1000,9 +1156,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.86459489650160992"/>
-          <c:y val="0.47634588537670092"/>
-          <c:w val="0.13096554606043792"/>
+          <c:x val="0.86459489650161003"/>
+          <c:y val="0.47634588537670097"/>
+          <c:w val="0.13096554606043795"/>
           <c:h val="6.3621571147249978E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -1124,8 +1280,8 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="60729600"/>
-        <c:axId val="60735488"/>
+        <c:axId val="36878592"/>
+        <c:axId val="36884480"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1214,11 +1370,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="60729600"/>
-        <c:axId val="60735488"/>
+        <c:axId val="36878592"/>
+        <c:axId val="36884480"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="60729600"/>
+        <c:axId val="36878592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1242,14 +1398,14 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60735488"/>
+        <c:crossAx val="36884480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60735488"/>
+        <c:axId val="36884480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1274,7 +1430,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60729600"/>
+        <c:crossAx val="36878592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1285,10 +1441,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.77880952380952573"/>
+          <c:x val="0.77880952380952584"/>
           <c:y val="0.38324174513150894"/>
           <c:w val="0.20690476190476192"/>
-          <c:h val="0.20622139015839863"/>
+          <c:h val="0.20622139015839869"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -1331,7 +1487,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1341,7 +1497,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Chart2"/>
   <sheetViews>
-    <sheetView zoomScale="106" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -3555,31 +3711,31 @@
       </c>
       <c r="H4" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>5.25</v>
       </c>
       <c r="I4" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J4" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K4" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L4" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M4" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N4" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O4" s="11" t="str">
         <f ca="1"/>
@@ -3975,11 +4131,11 @@
       </c>
       <c r="H5" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J5" s="11">
         <f ca="1"/>
@@ -4815,31 +4971,31 @@
       </c>
       <c r="H7" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="I7" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="J7" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="K7" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="L7" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="M7" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="N7" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="O7" s="11" t="str">
         <f ca="1"/>
@@ -5234,31 +5390,31 @@
       </c>
       <c r="H8" s="12">
         <f ca="1">IF('Sprint Information'!G$52,SUM(OFFSET(H$2,1,0,ROW()-3,1)),"")</f>
-        <v>0</v>
+        <v>10.75</v>
       </c>
       <c r="I8" s="12">
         <f ca="1">IF('Sprint Information'!H$52,SUM(OFFSET(I$2,1,0,ROW()-3,1)),"")</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J8" s="12">
         <f ca="1">IF('Sprint Information'!I$52,SUM(OFFSET(J$2,1,0,ROW()-3,1)),"")</f>
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="K8" s="12">
         <f ca="1">IF('Sprint Information'!J$52,SUM(OFFSET(K$2,1,0,ROW()-3,1)),"")</f>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="L8" s="12">
         <f ca="1">IF('Sprint Information'!K$52,SUM(OFFSET(L$2,1,0,ROW()-3,1)),"")</f>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="M8" s="12">
         <f ca="1">IF('Sprint Information'!L$52,SUM(OFFSET(M$2,1,0,ROW()-3,1)),"")</f>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="N8" s="12">
         <f ca="1">IF('Sprint Information'!M$52,SUM(OFFSET(N$2,1,0,ROW()-3,1)),"")</f>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="O8" s="12" t="str">
         <f ca="1">IF('Sprint Information'!N$52,SUM(OFFSET(O$2,1,0,ROW()-3,1)),"")</f>
@@ -5628,20 +5784,20 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C9:DA65536 C3:DA7">
-    <cfRule type="cellIs" dxfId="22" priority="1" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>C$1*Work_Hours_in_Day</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="2" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="34" priority="2" stopIfTrue="1" operator="lessThan">
       <formula>C$1*Work_Hours_in_Day</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:IV8">
-    <cfRule type="expression" dxfId="20" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="3" stopIfTrue="1">
       <formula>NOT(ISNUMBER(C$2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:XFD2">
-    <cfRule type="cellIs" dxfId="19" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="4" stopIfTrue="1" operator="equal">
       <formula>Sprint_Length + 1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5656,11 +5812,11 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:DE23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K19" sqref="K19"/>
+      <selection pane="bottomRight" activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelCol="1"/>
@@ -6552,13 +6708,27 @@
       <c r="K3" s="25">
         <v>0.5</v>
       </c>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="26"/>
-      <c r="R3" s="26"/>
+      <c r="L3" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="M3" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="N3" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="O3" s="26">
+        <v>0</v>
+      </c>
+      <c r="P3" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="26">
+        <v>0</v>
+      </c>
+      <c r="R3" s="26">
+        <v>0</v>
+      </c>
       <c r="S3" s="27"/>
       <c r="T3" s="27"/>
       <c r="U3" s="27"/>
@@ -6638,13 +6808,27 @@
       <c r="K5" s="25">
         <v>3</v>
       </c>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="25"/>
-      <c r="O5" s="28"/>
-      <c r="P5" s="28"/>
-      <c r="Q5" s="28"/>
-      <c r="R5" s="28"/>
+      <c r="L5" s="25">
+        <v>3</v>
+      </c>
+      <c r="M5" s="25">
+        <v>3</v>
+      </c>
+      <c r="N5" s="25">
+        <v>3</v>
+      </c>
+      <c r="O5" s="28">
+        <v>2.5</v>
+      </c>
+      <c r="P5" s="28">
+        <v>2.5</v>
+      </c>
+      <c r="Q5" s="28">
+        <v>2.5</v>
+      </c>
+      <c r="R5" s="28">
+        <v>2.5</v>
+      </c>
       <c r="S5" s="28"/>
       <c r="T5" s="28"/>
       <c r="U5" s="28"/>
@@ -6900,13 +7084,27 @@
       <c r="K11" s="25">
         <v>1</v>
       </c>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="25"/>
-      <c r="O11" s="28"/>
-      <c r="P11" s="28"/>
-      <c r="Q11" s="28"/>
-      <c r="R11" s="28"/>
+      <c r="L11" s="25">
+        <v>1</v>
+      </c>
+      <c r="M11" s="25">
+        <v>1</v>
+      </c>
+      <c r="N11" s="25">
+        <v>0</v>
+      </c>
+      <c r="O11" s="28">
+        <v>0</v>
+      </c>
+      <c r="P11" s="28">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="28">
+        <v>0</v>
+      </c>
+      <c r="R11" s="28">
+        <v>0</v>
+      </c>
       <c r="S11" s="29"/>
       <c r="T11" s="29"/>
       <c r="U11" s="29"/>
@@ -6936,13 +7134,27 @@
       <c r="K12" s="25">
         <v>0</v>
       </c>
-      <c r="L12" s="28"/>
-      <c r="M12" s="28"/>
-      <c r="N12" s="28"/>
-      <c r="O12" s="28"/>
-      <c r="P12" s="28"/>
-      <c r="Q12" s="28"/>
-      <c r="R12" s="28"/>
+      <c r="L12" s="28">
+        <v>0</v>
+      </c>
+      <c r="M12" s="28">
+        <v>0</v>
+      </c>
+      <c r="N12" s="28">
+        <v>0</v>
+      </c>
+      <c r="O12" s="28">
+        <v>0</v>
+      </c>
+      <c r="P12" s="28">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="28">
+        <v>0</v>
+      </c>
+      <c r="R12" s="28">
+        <v>0</v>
+      </c>
       <c r="S12" s="28"/>
       <c r="T12" s="28"/>
       <c r="U12" s="28"/>
@@ -6972,13 +7184,27 @@
       <c r="K13" s="25">
         <v>0.5</v>
       </c>
-      <c r="L13" s="25"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="25"/>
-      <c r="O13" s="28"/>
-      <c r="P13" s="28"/>
-      <c r="Q13" s="28"/>
-      <c r="R13" s="28"/>
+      <c r="L13" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="M13" s="25">
+        <v>0</v>
+      </c>
+      <c r="N13" s="25">
+        <v>0</v>
+      </c>
+      <c r="O13" s="28">
+        <v>0</v>
+      </c>
+      <c r="P13" s="28">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="28">
+        <v>0</v>
+      </c>
+      <c r="R13" s="28">
+        <v>0</v>
+      </c>
       <c r="S13" s="28"/>
       <c r="T13" s="28"/>
       <c r="U13" s="28"/>
@@ -7158,13 +7384,27 @@
       <c r="K17" s="25">
         <v>0.5</v>
       </c>
-      <c r="L17" s="25"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="25"/>
-      <c r="O17" s="25"/>
-      <c r="P17" s="25"/>
-      <c r="Q17" s="28"/>
-      <c r="R17" s="28"/>
+      <c r="L17" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="M17" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="N17" s="25">
+        <v>0</v>
+      </c>
+      <c r="O17" s="25">
+        <v>0</v>
+      </c>
+      <c r="P17" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="28">
+        <v>0</v>
+      </c>
+      <c r="R17" s="28">
+        <v>0</v>
+      </c>
       <c r="S17" s="28"/>
       <c r="T17" s="28"/>
       <c r="U17" s="28"/>
@@ -7189,16 +7429,30 @@
       <c r="J18" s="25">
         <v>5</v>
       </c>
-      <c r="K18" s="25">
-        <v>5</v>
-      </c>
-      <c r="L18" s="25"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="25"/>
-      <c r="O18" s="25"/>
-      <c r="P18" s="25"/>
-      <c r="Q18" s="28"/>
-      <c r="R18" s="28"/>
+      <c r="K18" s="28">
+        <v>4.5</v>
+      </c>
+      <c r="L18" s="28">
+        <v>4.5</v>
+      </c>
+      <c r="M18" s="28">
+        <v>4.5</v>
+      </c>
+      <c r="N18" s="28">
+        <v>4.5</v>
+      </c>
+      <c r="O18" s="28">
+        <v>4.5</v>
+      </c>
+      <c r="P18" s="28">
+        <v>4.5</v>
+      </c>
+      <c r="Q18" s="28">
+        <v>4.5</v>
+      </c>
+      <c r="R18" s="28">
+        <v>4.5</v>
+      </c>
       <c r="S18" s="28"/>
       <c r="T18" s="28"/>
       <c r="U18" s="28"/>
@@ -7228,13 +7482,27 @@
       <c r="K19" s="25">
         <v>5.25</v>
       </c>
-      <c r="L19" s="25"/>
-      <c r="M19" s="25"/>
-      <c r="N19" s="25"/>
-      <c r="O19" s="28"/>
-      <c r="P19" s="28"/>
-      <c r="Q19" s="28"/>
-      <c r="R19" s="28"/>
+      <c r="L19" s="25">
+        <v>5.25</v>
+      </c>
+      <c r="M19" s="25">
+        <v>4</v>
+      </c>
+      <c r="N19" s="25">
+        <v>4</v>
+      </c>
+      <c r="O19" s="25">
+        <v>4</v>
+      </c>
+      <c r="P19" s="28">
+        <v>4</v>
+      </c>
+      <c r="Q19" s="28">
+        <v>4</v>
+      </c>
+      <c r="R19" s="28">
+        <v>4</v>
+      </c>
       <c r="S19" s="28"/>
       <c r="T19" s="28"/>
       <c r="U19" s="28"/>
@@ -7321,71 +7589,101 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B24:B65536 B7:B21">
-    <cfRule type="expression" dxfId="18" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="10" stopIfTrue="1">
       <formula>IF($F7=INDEX(Postponed_Values,1,1),TRUE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="11" stopIfTrue="1">
       <formula>IF(ISBLANK($G7),FALSE,OFFSET($G7,0,COUNT($G7:$DE7)-1)=0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G24:T65536 O22:T22 O19:P20 U3:DE65536 T3:T20 O3:S5 S7:S20 Q11:R20 O7:R8 O11:P16">
-    <cfRule type="expression" dxfId="16" priority="6" stopIfTrue="1">
+  <conditionalFormatting sqref="G24:T65536 O22:T22 O11:P16 U3:DE65536 T3:T20 O3:S5 S7:S20 O7:R8 P19:P20 O20 Q11:R20">
+    <cfRule type="expression" dxfId="29" priority="12" stopIfTrue="1">
       <formula>AND($F3=INDEX(Postponed_Values,1,1),ISNUMBER(G$1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:B2 D2:IV2">
-    <cfRule type="cellIs" dxfId="15" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="13" stopIfTrue="1" operator="equal">
       <formula>Sprint_Length + 1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="expression" dxfId="14" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="14" stopIfTrue="1">
       <formula>AND(ISBLANK($C1),ISNUMBER($G1))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="15" stopIfTrue="1">
       <formula>AND(VLOOKUP($C1,Commitment,3,FALSE)&gt;0,VLOOKUP($C1,Commitment,3,FALSE)&lt;&gt;"")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="16" stopIfTrue="1">
       <formula>AND(VLOOKUP($C1,Commitment,3,FALSE)&lt;0,VLOOKUP($C1,Commitment,3,FALSE)&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="expression" dxfId="11" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="19" stopIfTrue="1">
       <formula>IF($F4=INDEX(Postponed_Values,1,1),TRUE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="20" stopIfTrue="1">
       <formula>IF(ISBLANK($G4),FALSE,OFFSET($G4,0,COUNT($G4:$DE4)-1)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="expression" dxfId="9" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="23" stopIfTrue="1">
       <formula>IF($F11=INDEX(Postponed_Values,1,1),TRUE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="24" stopIfTrue="1">
       <formula>IF(ISBLANK($G11),FALSE,OFFSET($G11,0,COUNT($G11:$DE11)-1)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B6">
-    <cfRule type="expression" dxfId="7" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="27" stopIfTrue="1">
       <formula>IF($F22=INDEX(Postponed_Values,1,1),TRUE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="28" stopIfTrue="1">
       <formula>IF(ISBLANK($G22),FALSE,OFFSET($G22,0,COUNT($G22:$DE22)-1)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N12">
-    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="9" stopIfTrue="1">
       <formula>AND($F12=INDEX(Postponed_Values,1,1),ISNUMBER(N$1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M12">
-    <cfRule type="expression" dxfId="4" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="8" stopIfTrue="1">
       <formula>AND($F12=INDEX(Postponed_Values,1,1),ISNUMBER(M$1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L12">
-    <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="7" stopIfTrue="1">
       <formula>AND($F12=INDEX(Postponed_Values,1,1),ISNUMBER(L$1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P18">
+    <cfRule type="expression" dxfId="11" priority="6" stopIfTrue="1">
+      <formula>AND($F18=INDEX(Postponed_Values,1,1),ISNUMBER(P$1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O18">
+    <cfRule type="expression" dxfId="9" priority="5" stopIfTrue="1">
+      <formula>AND($F18=INDEX(Postponed_Values,1,1),ISNUMBER(O$1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N18">
+    <cfRule type="expression" dxfId="7" priority="4" stopIfTrue="1">
+      <formula>AND($F18=INDEX(Postponed_Values,1,1),ISNUMBER(N$1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18">
+    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
+      <formula>AND($F18=INDEX(Postponed_Values,1,1),ISNUMBER(K$1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L18">
+    <cfRule type="expression" dxfId="3" priority="2" stopIfTrue="1">
+      <formula>AND($F18=INDEX(Postponed_Values,1,1),ISNUMBER(L$1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M18">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+      <formula>AND($F18=INDEX(Postponed_Values,1,1),ISNUMBER(M$1))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
@@ -9260,7 +9558,7 @@
       </c>
       <c r="C4" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D4" s="11">
         <f t="array" ref="D4:DB4" ca="1">IF(ROW()&gt;COUNTA(Resource)+3,"",IF(Held_Standup,IF(ROW()=COUNTA(Resource)+3,SUM(INDEX(OFFSET($D$2,1,0,ROW()-3,Sprint_Length+1),0,COLUMN()-3)),OFFSET('Resource Allocation'!$C$2,INDEX(ROW(),1,1)-2,0,1,103)*OFFSET('Resource Allocation'!$A$2,INDEX(ROW(),1,1)-2,0)),""))</f>
@@ -9284,31 +9582,31 @@
       </c>
       <c r="I4" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>5.25</v>
       </c>
       <c r="J4" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K4" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L4" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M4" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N4" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O4" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P4" s="11" t="str">
         <f ca="1"/>
@@ -9710,11 +10008,11 @@
       </c>
       <c r="I5" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K5" s="11">
         <f ca="1"/>
@@ -10538,7 +10836,7 @@
       </c>
       <c r="C7" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="D7" s="11">
         <f t="array" ref="D7:DB7" ca="1">IF(ROW()&gt;COUNTA(Resource)+3,"",IF(Held_Standup,IF(ROW()=COUNTA(Resource)+3,SUM(INDEX(OFFSET($D$2,1,0,ROW()-3,Sprint_Length+1),0,COLUMN()-3)),OFFSET('Resource Allocation'!$C$2,INDEX(ROW(),1,1)-2,0,1,103)*OFFSET('Resource Allocation'!$A$2,INDEX(ROW(),1,1)-2,0)),""))</f>
@@ -10562,31 +10860,31 @@
       </c>
       <c r="I7" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="J7" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="K7" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="L7" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="M7" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="N7" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="O7" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="P7" s="11" t="str">
         <f ca="1"/>
@@ -10988,31 +11286,31 @@
       </c>
       <c r="I8" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>10.75</v>
       </c>
       <c r="J8" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="K8" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="L8" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="M8" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="N8" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="O8" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="P8" s="11" t="str">
         <f ca="1"/>
@@ -22030,15 +22328,15 @@
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="D2:IV2">
-    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="3" stopIfTrue="1" operator="equal">
       <formula>Sprint_Length+1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:DB65536">
-    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>D$1*Work_Hours_in_Day*OFFSET(Resource,MATCH($A3,Resource,0)-1,-1,1,1)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="2" stopIfTrue="1" operator="lessThan">
       <formula>D$1*Work_Hours_in_Day*OFFSET(Resource,MATCH($A3,Resource,0)-1,-1,1,1)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
diverse aktualisierungen + präsi
präsi, update user stories, burndown chart aktualisiert,
architekturdiagramm angefertigt
</commit_message>
<xml_diff>
--- a/Dokumentation/MS5/Burndown.xlsx
+++ b/Dokumentation/MS5/Burndown.xlsx
@@ -391,18 +391,41 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="29">
     <dxf>
       <font>
-        <strike val="0"/>
+        <b/>
+        <i val="0"/>
         <condense val="0"/>
         <extend val="0"/>
+        <color indexed="17"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="26"/>
-        </patternFill>
-      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -475,113 +498,6 @@
           <bgColor indexed="26"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="26"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="26"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="26"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="26"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="26"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="26"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="17"/>
-      </font>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="9"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -771,7 +687,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="de-DE" baseline="0"/>
-              <a:t>chart - Iteration 4 - Gruppe 1</a:t>
+              <a:t>chart - Iteration 5 - Gruppe 1</a:t>
             </a:r>
             <a:endParaRPr lang="de-DE"/>
           </a:p>
@@ -781,8 +697,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38247699037620397"/>
-          <c:y val="1.9575856443719442E-2"/>
+          <c:x val="0.38247699037620408"/>
+          <c:y val="1.9575856443719446E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -800,8 +716,8 @@
           <c:yMode val="edge"/>
           <c:x val="6.3263041065482792E-2"/>
           <c:y val="0.11092985318107668"/>
-          <c:w val="0.78912319644839213"/>
-          <c:h val="0.79282218597063425"/>
+          <c:w val="0.78912319644839224"/>
+          <c:h val="0.79282218597063403"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -973,11 +889,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="36675968"/>
-        <c:axId val="36678272"/>
+        <c:axId val="34676736"/>
+        <c:axId val="34679424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="36675968"/>
+        <c:axId val="34676736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1047,7 +963,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36678272"/>
+        <c:crossAx val="34679424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1056,7 +972,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="36678272"/>
+        <c:axId val="34679424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1099,7 +1015,7 @@
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
               <c:x val="1.2208724689406945E-2"/>
-              <c:y val="0.43230022178461258"/>
+              <c:y val="0.43230022178461269"/>
             </c:manualLayout>
           </c:layout>
           <c:spPr>
@@ -1136,7 +1052,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36675968"/>
+        <c:crossAx val="34676736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1156,9 +1072,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.86459489650161003"/>
-          <c:y val="0.47634588537670097"/>
-          <c:w val="0.13096554606043795"/>
+          <c:x val="0.86459489650161014"/>
+          <c:y val="0.47634588537670103"/>
+          <c:w val="0.13096554606043798"/>
           <c:h val="6.3621571147249978E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -1280,8 +1196,8 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="36878592"/>
-        <c:axId val="36884480"/>
+        <c:axId val="35428608"/>
+        <c:axId val="35434496"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1370,11 +1286,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="36878592"/>
-        <c:axId val="36884480"/>
+        <c:axId val="35428608"/>
+        <c:axId val="35434496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="36878592"/>
+        <c:axId val="35428608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1398,14 +1314,14 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36884480"/>
+        <c:crossAx val="35434496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="36884480"/>
+        <c:axId val="35434496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1430,7 +1346,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36878592"/>
+        <c:crossAx val="35428608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1441,10 +1357,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.77880952380952584"/>
+          <c:x val="0.77880952380952595"/>
           <c:y val="0.38324174513150894"/>
           <c:w val="0.20690476190476192"/>
-          <c:h val="0.20622139015839869"/>
+          <c:h val="0.20622139015839874"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -1487,7 +1403,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5784,20 +5700,20 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C9:DA65536 C3:DA7">
-    <cfRule type="cellIs" dxfId="35" priority="1" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>C$1*Work_Hours_in_Day</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="2" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="27" priority="2" stopIfTrue="1" operator="lessThan">
       <formula>C$1*Work_Hours_in_Day</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:IV8">
-    <cfRule type="expression" dxfId="33" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="3" stopIfTrue="1">
       <formula>NOT(ISNUMBER(C$2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:XFD2">
-    <cfRule type="cellIs" dxfId="32" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="4" stopIfTrue="1" operator="equal">
       <formula>Sprint_Length + 1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7589,85 +7505,85 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B24:B65536 B7:B21">
-    <cfRule type="expression" dxfId="31" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="10" stopIfTrue="1">
       <formula>IF($F7=INDEX(Postponed_Values,1,1),TRUE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="11" stopIfTrue="1">
       <formula>IF(ISBLANK($G7),FALSE,OFFSET($G7,0,COUNT($G7:$DE7)-1)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G24:T65536 O22:T22 O11:P16 U3:DE65536 T3:T20 O3:S5 S7:S20 O7:R8 P19:P20 O20 Q11:R20">
-    <cfRule type="expression" dxfId="29" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="12" stopIfTrue="1">
       <formula>AND($F3=INDEX(Postponed_Values,1,1),ISNUMBER(G$1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:B2 D2:IV2">
-    <cfRule type="cellIs" dxfId="28" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="13" stopIfTrue="1" operator="equal">
       <formula>Sprint_Length + 1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="expression" dxfId="27" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="14" stopIfTrue="1">
       <formula>AND(ISBLANK($C1),ISNUMBER($G1))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="15" stopIfTrue="1">
       <formula>AND(VLOOKUP($C1,Commitment,3,FALSE)&gt;0,VLOOKUP($C1,Commitment,3,FALSE)&lt;&gt;"")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="16" stopIfTrue="1">
       <formula>AND(VLOOKUP($C1,Commitment,3,FALSE)&lt;0,VLOOKUP($C1,Commitment,3,FALSE)&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="expression" dxfId="24" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="19" stopIfTrue="1">
       <formula>IF($F4=INDEX(Postponed_Values,1,1),TRUE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="20" stopIfTrue="1">
       <formula>IF(ISBLANK($G4),FALSE,OFFSET($G4,0,COUNT($G4:$DE4)-1)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="expression" dxfId="22" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="23" stopIfTrue="1">
       <formula>IF($F11=INDEX(Postponed_Values,1,1),TRUE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="24" stopIfTrue="1">
       <formula>IF(ISBLANK($G11),FALSE,OFFSET($G11,0,COUNT($G11:$DE11)-1)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B6">
-    <cfRule type="expression" dxfId="20" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="27" stopIfTrue="1">
       <formula>IF($F22=INDEX(Postponed_Values,1,1),TRUE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="28" stopIfTrue="1">
       <formula>IF(ISBLANK($G22),FALSE,OFFSET($G22,0,COUNT($G22:$DE22)-1)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N12">
-    <cfRule type="expression" dxfId="18" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="9" stopIfTrue="1">
       <formula>AND($F12=INDEX(Postponed_Values,1,1),ISNUMBER(N$1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M12">
-    <cfRule type="expression" dxfId="17" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="8" stopIfTrue="1">
       <formula>AND($F12=INDEX(Postponed_Values,1,1),ISNUMBER(M$1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L12">
-    <cfRule type="expression" dxfId="16" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="7" stopIfTrue="1">
       <formula>AND($F12=INDEX(Postponed_Values,1,1),ISNUMBER(L$1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P18">
-    <cfRule type="expression" dxfId="11" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="6" stopIfTrue="1">
       <formula>AND($F18=INDEX(Postponed_Values,1,1),ISNUMBER(P$1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O18">
-    <cfRule type="expression" dxfId="9" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="5" stopIfTrue="1">
       <formula>AND($F18=INDEX(Postponed_Values,1,1),ISNUMBER(O$1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N18">
-    <cfRule type="expression" dxfId="7" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="4" stopIfTrue="1">
       <formula>AND($F18=INDEX(Postponed_Values,1,1),ISNUMBER(N$1))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7677,12 +7593,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L18">
-    <cfRule type="expression" dxfId="3" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="2" stopIfTrue="1">
       <formula>AND($F18=INDEX(Postponed_Values,1,1),ISNUMBER(L$1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M18">
-    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
       <formula>AND($F18=INDEX(Postponed_Values,1,1),ISNUMBER(M$1))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22328,15 +22244,15 @@
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="D2:IV2">
-    <cfRule type="cellIs" dxfId="15" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="equal">
       <formula>Sprint_Length+1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:DB65536">
-    <cfRule type="cellIs" dxfId="14" priority="1" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>D$1*Work_Hours_in_Day*OFFSET(Resource,MATCH($A3,Resource,0)-1,-1,1,1)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="2" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="lessThan">
       <formula>D$1*Work_Hours_in_Day*OFFSET(Resource,MATCH($A3,Resource,0)-1,-1,1,1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24961,9 +24877,9 @@
       <c r="A60" t="s">
         <v>28</v>
       </c>
-      <c r="B60" t="str">
+      <c r="B60" t="e">
         <f ca="1">MID(CELL("filename"),FIND("[",CELL("filename"))+1,FIND("]",CELL("filename"))-FIND("[",CELL("filename"))-IF(MID(CELL("filename"),FIND("]",CELL("filename"))-4,1)=".",5,6))</f>
-        <v>Burndown</v>
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>

</xml_diff>